<commit_message>
Add 0.0.0.0 to app.listen, update bug report
</commit_message>
<xml_diff>
--- a/client/public/bugs/BugReport_250507.xlsx
+++ b/client/public/bugs/BugReport_250507.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -281,6 +281,21 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1633,255 +1648,615 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="3" max="4" width="29.57421875"/>
-    <col customWidth="1" min="8" max="8" width="40.00390625"/>
+    <col customWidth="1" min="3" max="3" style="17" width="29.57421875"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="9.140625"/>
+    <col bestFit="1" min="5" max="5" width="9.28125"/>
+    <col customWidth="1" min="8" max="8" style="17" width="47.140625"/>
+    <col customWidth="1" min="9" max="9" style="18" width="30.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
+      <c r="A1" s="6" t="str">
+        <f>Sheet1!A1</f>
+        <v>Order</v>
+      </c>
+      <c r="B1" s="6" t="str">
+        <f>Sheet1!B1</f>
+        <v>Category</v>
+      </c>
+      <c r="C1" s="19" t="str">
+        <f>Sheet1!C1</f>
+        <v xml:space="preserve">App Location</v>
+      </c>
+      <c r="D1" s="6" t="str">
+        <f>Sheet1!D1</f>
+        <v>Priority</v>
+      </c>
+      <c r="E1" s="6" t="str">
+        <f>Sheet1!E1</f>
+        <v>Severity</v>
+      </c>
+      <c r="F1" s="6" t="str">
+        <f>Sheet1!F1</f>
+        <v>LOE</v>
+      </c>
+      <c r="G1" s="6" t="str">
+        <f>Sheet1!G1</f>
+        <v>Effects</v>
+      </c>
+      <c r="H1" s="19" t="str">
+        <f>Sheet1!H1</f>
+        <v>Description</v>
+      </c>
+      <c r="I1" s="20" t="str">
+        <f>Sheet1!I1</f>
+        <v>Solution</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
+        <f>Sheet1!A2</f>
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="B2" s="2" t="str">
+        <f>Sheet1!B2</f>
+        <v>Bug</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f>Sheet1!C2</f>
+        <v>Mobile</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>Sheet1!D2</f>
+        <v>High</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>Sheet1!E2</f>
+        <v>Critical</v>
+      </c>
+      <c r="F2" s="2">
+        <f>Sheet1!F2</f>
         <v>8</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
+      <c r="G2" s="2"/>
+      <c r="H2" s="16" t="str">
+        <f>Sheet1!H2</f>
+        <v xml:space="preserve">Login does not work</v>
+      </c>
+      <c r="I2" s="21" t="str">
+        <f>Sheet1!I2</f>
+        <v>Mike</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
+        <f>Sheet1!A3</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="B3" s="2" t="str">
+        <f>Sheet1!B3</f>
+        <v>Bug</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f>Sheet1!C3</f>
+        <v xml:space="preserve">Reaction Dialog</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>Sheet1!D3</f>
+        <v>Medium</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>Sheet1!E3</f>
+        <v>High</v>
+      </c>
+      <c r="F3" s="2">
+        <f>Sheet1!F3</f>
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" ht="42.75">
+      <c r="G3" s="2" t="str">
+        <f>Sheet1!G3</f>
+        <v>Mike</v>
+      </c>
+      <c r="H3" s="16" t="str">
+        <f>Sheet1!H3</f>
+        <v xml:space="preserve">Incorrect location displayed</v>
+      </c>
+      <c r="I3" s="21" t="str">
+        <f>Sheet1!I3</f>
+        <v>Mike</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="2">
+        <f>Sheet1!A4</f>
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="B4" s="2" t="str">
+        <f>Sheet1!B4</f>
+        <v>Bug</v>
+      </c>
+      <c r="C4" s="16" t="str">
+        <f>Sheet1!C4</f>
+        <v xml:space="preserve">All video views</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>Sheet1!D4</f>
+        <v>Medium</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f>Sheet1!E4</f>
+        <v>Medium</v>
+      </c>
+      <c r="F4" s="2">
+        <f>Sheet1!F4</f>
         <v>5</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" ht="28.5">
+      <c r="G4" s="2"/>
+      <c r="H4" s="16" t="str">
+        <f>Sheet1!H4</f>
+        <v xml:space="preserve">Blank videos
+(Related to 4?)
+</v>
+      </c>
+      <c r="I4" s="21" t="str">
+        <f>Sheet1!I4</f>
+        <v>Mike</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="2">
+        <f>Sheet1!A5</f>
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="B5" s="2" t="str">
+        <f>Sheet1!B5</f>
+        <v>Bug</v>
+      </c>
+      <c r="C5" s="16" t="str">
+        <f>Sheet1!C5</f>
+        <v>Everywhere</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>Sheet1!D5</f>
+        <v>Medium?</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>Sheet1!E5</f>
+        <v>Uncertain</v>
+      </c>
+      <c r="F5" s="2">
+        <f>Sheet1!F5</f>
         <v>5</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="G5" s="2"/>
+      <c r="H5" s="16" t="str">
+        <f>Sheet1!H5</f>
+        <v xml:space="preserve">Many 404 for videos
+(Related to 3?)</v>
+      </c>
+      <c r="I5" s="21" t="str">
+        <f>Sheet1!I5</f>
+        <v>Mike</v>
+      </c>
+    </row>
+    <row r="6" ht="71.25">
       <c r="A6" s="2">
+        <f>Sheet1!A6</f>
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>32</v>
+      <c r="B6" s="2" t="str">
+        <f>Sheet1!B6</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C6" s="16" t="str">
+        <f>Sheet1!C6</f>
+        <v>Frontpage</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>Sheet1!D6</f>
+        <v>High</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>Sheet1!E6</f>
+        <v>Low</v>
+      </c>
+      <c r="F6" s="2">
+        <f>Sheet1!F6</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="16" t="str">
+        <f>Sheet1!H6</f>
+        <v xml:space="preserve">Forntpage to display highest ranking videos</v>
+      </c>
+      <c r="I6" s="21" t="str">
+        <f>Sheet1!I6</f>
+        <v xml:space="preserve">Fake It?
+After rename: top three to be 032_20250411T041956937Z.mp4
+089_20250411T041955185Z.mp4
+132_20250402T18350000Z.mp4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>33</v>
+        <f>Sheet1!A7</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>Sheet1!B7</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C7" s="16" t="str">
+        <f>Sheet1!C7</f>
+        <v>Tab</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>Sheet1!D7</f>
+        <v>Low</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2">
+        <f>Sheet1!F7</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="16" t="str">
+        <f>Sheet1!H7</f>
+        <v xml:space="preserve">Fix favicon</v>
+      </c>
+      <c r="I7" s="21" t="str">
+        <f>Sheet1!I7</f>
+        <v>Mike</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>35</v>
+        <f>Sheet1!A8</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>Sheet1!B8</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C8" s="16" t="str">
+        <f>Sheet1!C8</f>
+        <v>Mobile</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>Sheet1!D8</f>
+        <v>Low</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="16" t="str">
+        <f>Sheet1!H8</f>
+        <v xml:space="preserve">Menu spacing</v>
+      </c>
+      <c r="I8" s="21">
+        <f>Sheet1!I8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
+        <f>Sheet1!A9</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>Sheet1!B9</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C9" s="16" t="str">
+        <f>Sheet1!C9</f>
+        <v xml:space="preserve">Camera list in Gallery</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>Sheet1!D9</f>
+        <v>Low</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="16" t="str">
+        <f>Sheet1!H9</f>
+        <v xml:space="preserve">Sort order</v>
+      </c>
+      <c r="I9" s="21">
+        <f>Sheet1!I9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <f>Sheet1!A10</f>
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" ht="28.5">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>39</v>
+      <c r="B10" s="2" t="str">
+        <f>Sheet1!B10</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C10" s="16" t="str">
+        <f>Sheet1!C10</f>
+        <v xml:space="preserve">Social Media Icons and Links</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>Sheet1!D10</f>
+        <v>Low</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="16" t="str">
+        <f>Sheet1!H10</f>
+        <v xml:space="preserve">Not consistent on pages and reaction dialog</v>
+      </c>
+      <c r="I10" s="21">
+        <f>Sheet1!I10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
+        <f>Sheet1!A11</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>Sheet1!B11</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C11" s="16" t="str">
+        <f>Sheet1!C11</f>
+        <v xml:space="preserve">Mobile Frontpage</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>Sheet1!D11</f>
+        <v>Low</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="16" t="str">
+        <f>Sheet1!H11</f>
+        <v xml:space="preserve">Display does not scroll to bottom of video stack</v>
+      </c>
+      <c r="I11" s="21">
+        <f>Sheet1!I11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <f>Sheet1!A12</f>
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="B12" s="2" t="str">
+        <f>Sheet1!B12</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C12" s="16" t="str">
+        <f>Sheet1!C12</f>
+        <v xml:space="preserve">Reaction dialog</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>Sheet1!D12</f>
+        <v>Low</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="16" t="str">
+        <f>Sheet1!H12</f>
+        <v xml:space="preserve">Add close button</v>
+      </c>
+      <c r="I12" s="21">
+        <f>Sheet1!I12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <f>Sheet1!A13</f>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>Sheet1!B13</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C13" s="16" t="str">
+        <f>Sheet1!C13</f>
+        <v>Frontpage</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f>Sheet1!D13</f>
+        <v>Low</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="16" t="str">
+        <f>Sheet1!H13</f>
+        <v xml:space="preserve">Show Likes count and Star icon</v>
+      </c>
+      <c r="I13" s="21">
+        <f>Sheet1!I13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <f>Sheet1!A14</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>Sheet1!B14</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C14" s="16" t="str">
+        <f>Sheet1!C14</f>
+        <v>Everywhere</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f>Sheet1!D14</f>
+        <v>Low</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="16" t="str">
+        <f>Sheet1!H14</f>
+        <v xml:space="preserve">Make subheadings yellow for contrast</v>
+      </c>
+      <c r="I14" s="21">
+        <f>Sheet1!I14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <f>Sheet1!A15</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>Sheet1!B15</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C15" s="16" t="str">
+        <f>Sheet1!C15</f>
+        <v>Everywhere</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f>Sheet1!D15</f>
+        <v>Low</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="16" t="str">
+        <f>Sheet1!H15</f>
+        <v xml:space="preserve">Select better images</v>
+      </c>
+      <c r="I15" s="21">
+        <f>Sheet1!I15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <f>Sheet1!A16</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>Sheet1!B16</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C16" s="16" t="str">
+        <f>Sheet1!C16</f>
+        <v>Frontpage</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f>Sheet1!D16</f>
+        <v>Medium</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="16" t="str">
+        <f>Sheet1!H16</f>
+        <v xml:space="preserve">Add instructions to popout on hover or menu</v>
+      </c>
+      <c r="I16" s="21">
+        <f>Sheet1!I16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <f>Sheet1!A17</f>
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>Sheet1!B17</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C17" s="16" t="str">
+        <f>Sheet1!C17</f>
+        <v>Frontpage</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>Sheet1!D17</f>
+        <v>Low</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="16" t="str">
+        <f>Sheet1!H17</f>
+        <v xml:space="preserve">Change "Top 3 Most Liked Videos" to "Top Videos"</v>
+      </c>
+      <c r="I17" s="21">
+        <f>Sheet1!I17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <f>Sheet1!A18</f>
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>Sheet1!B18</f>
+        <v>Tweak</v>
+      </c>
+      <c r="C18" s="16" t="str">
+        <f>Sheet1!C18</f>
+        <v>Frontpage</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f>Sheet1!D18</f>
+        <v>Low</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="16" t="str">
+        <f>Sheet1!H18</f>
+        <v xml:space="preserve">Display entire page by default</v>
+      </c>
+      <c r="I18" s="21" t="str">
+        <f>Sheet1!I18</f>
+        <v xml:space="preserve">Workaround: F11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="19"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="19"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>